<commit_message>
Updated Data Excel and added a Summary Excel
</commit_message>
<xml_diff>
--- a/Documentation/Data.xlsx
+++ b/Documentation/Data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17127"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jairu\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angelicalaurene\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="118">
   <si>
     <t>Name</t>
   </si>
@@ -44,15 +44,9 @@
     <t>Steps:</t>
   </si>
   <si>
-    <t>Have you experienced pre-registering</t>
-  </si>
-  <si>
     <t>Are you satisfied?</t>
   </si>
   <si>
-    <t>Comments:</t>
-  </si>
-  <si>
     <t>Enrico Gloria</t>
   </si>
   <si>
@@ -261,13 +255,136 @@
   </si>
   <si>
     <t>There should be a better system on figuring out how many classes/slots to open so everyone can be accomodated, pero di naman sobrang lala ng ganitong cases sa amin</t>
+  </si>
+  <si>
+    <t>Eva Ramoso Samillano</t>
+  </si>
+  <si>
+    <t>APC</t>
+  </si>
+  <si>
+    <t>BSCS-SS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Merong pinapafill up na form 2) Check yung Masters List sa FLAVIO kung available yung subject na gusto mo 3) Kunin mo schedule ng adviser na magssign sa form mo 4) Magpa-sign ng form </t>
+  </si>
+  <si>
+    <t xml:space="preserve">No, kasi pag nagpapa-preregister, hassle dahil kumpulan sa pagpapapirma </t>
+  </si>
+  <si>
+    <t>Di maayos yung pagkaka-schedule sa pag pre-register</t>
+  </si>
+  <si>
+    <t>Samantha Galeon Mallari</t>
+  </si>
+  <si>
+    <t>RATE YOUR SATISFACTION (1 - 5) 1 being the lowest and 5 being the highest</t>
+  </si>
+  <si>
+    <t>1) Kuha ka ng form sa registrar 2) Check yung course code sa Masters List 3) Fill up mo yung form 4) Wait in line sa adviser 5) Bigay sa adviser yung form 6) Pirmahan ng adviser yung form 7) Ibabalik sayo yung form with signature</t>
+  </si>
+  <si>
+    <t>Di masyado</t>
+  </si>
+  <si>
+    <t>Comments/Recommendations/Suggestions/Violent Reactions:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pag nag ppregister kasi, yung mga tao napipilitan na madaliin yung pagpili ng subject (sa elective) kasi nga agawan sa slots. Mas maganda kung lahat may equal chances sa pagkuha ng subject by randomizing pero sa elective. </t>
+  </si>
+  <si>
+    <t>Paulo Miguel Sinsin Capuz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1) Kuha form sa registrar 2) Maghanap ng designated prof para sa prereg 3) Magpre-register </t>
+  </si>
+  <si>
+    <t>Very unsatisfied</t>
+  </si>
+  <si>
+    <t>nakakapagod maghintay</t>
+  </si>
+  <si>
+    <t>Faith Ballesteros</t>
+  </si>
+  <si>
+    <t>First. Get a copy of the pre registration paper from the registrar. Second, look for the designated professor.</t>
+  </si>
+  <si>
+    <t>The experience was exhausting and tiring. If there is only an automated pre registration system then students won't have to go through that.</t>
+  </si>
+  <si>
+    <t>Rolando Aurelio Talag</t>
+  </si>
+  <si>
+    <t>Step 1- Present your ID then get a copy reg. paper from the registrar. Step 2- fill up the reg. form and bring to the encoder.</t>
+  </si>
+  <si>
+    <t>Very unstisfied</t>
+  </si>
+  <si>
+    <t>Please fix proper scheduling of encoder.</t>
+  </si>
+  <si>
+    <t>Genesis Diocampo</t>
+  </si>
+  <si>
+    <t>Unsatisfied</t>
+  </si>
+  <si>
+    <t>Sayang oras dahil madami pang pinupuntahan</t>
+  </si>
+  <si>
+    <t>Denzel F. Oribiana</t>
+  </si>
+  <si>
+    <t>BSCS-ss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Time is wasted because of the manual system,last time I registered a subject, it took about 1 and a half hour. </t>
+  </si>
+  <si>
+    <t>Jesus P. Brugada</t>
+  </si>
+  <si>
+    <t>Ang tagal magsimula at matapos, then ang haba pa ng pilam sobrang unorganized tuwing pre-reg</t>
+  </si>
+  <si>
+    <t>Fons Tison</t>
+  </si>
+  <si>
+    <t>Yeah</t>
+  </si>
+  <si>
+    <t>yeah</t>
+  </si>
+  <si>
+    <t>(Same steps as above)</t>
+  </si>
+  <si>
+    <t>Nagrereklamo yung ibang mga prof na nakakakita sa haba ng pila ng pre-reg. Dapat sisihin nila yung sistema, hindi ung mga estudyanteng gusto makakuha ng subject na gusto nila.</t>
+  </si>
+  <si>
+    <t>Jefferson Gonzales</t>
+  </si>
+  <si>
+    <t>Hassle yung prereg nila kasi pupunta pa sa 4th floor para magprepreg, aapproach pa natin personally yung mga designated prof na magaapprove. Massuggest ko na tayo na mismong students mag add ng subjects ng online.</t>
+  </si>
+  <si>
+    <t>Year Level</t>
+  </si>
+  <si>
+    <t>3rd Yr College</t>
+  </si>
+  <si>
+    <t>Have you experienced pre-registering?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -275,13 +392,27 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -296,7 +427,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -304,11 +435,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="13">
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -319,6 +524,26 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:K24" totalsRowShown="0" headerRowDxfId="11" dataDxfId="12">
+  <autoFilter ref="A1:K24"/>
+  <tableColumns count="11">
+    <tableColumn id="1" name="Name" dataDxfId="10"/>
+    <tableColumn id="2" name="School" dataDxfId="9"/>
+    <tableColumn id="3" name="Course" dataDxfId="8"/>
+    <tableColumn id="12" name="Year Level" dataDxfId="7"/>
+    <tableColumn id="4" name="Do you have a pre-registration system in your school?" dataDxfId="6"/>
+    <tableColumn id="5" name="Online or Manual?" dataDxfId="5"/>
+    <tableColumn id="6" name="Steps:" dataDxfId="4"/>
+    <tableColumn id="7" name="Have you experienced pre-registering?" dataDxfId="3"/>
+    <tableColumn id="8" name="Are you satisfied?" dataDxfId="2"/>
+    <tableColumn id="9" name="Comments/Recommendations/Suggestions/Violent Reactions:" dataDxfId="0"/>
+    <tableColumn id="10" name="RATE YOUR SATISFACTION (1 - 5) 1 being the lowest and 5 being the highest" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -618,403 +843,793 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
-    <col min="4" max="4" width="38" customWidth="1"/>
-    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="5" max="5" width="19.5703125" customWidth="1"/>
     <col min="6" max="6" width="34.42578125" customWidth="1"/>
-    <col min="7" max="7" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="36.5703125" customWidth="1"/>
     <col min="8" max="8" width="21.85546875" customWidth="1"/>
-    <col min="9" max="9" width="12.85546875" customWidth="1"/>
+    <col min="9" max="9" width="58.5703125" customWidth="1"/>
+    <col min="10" max="10" width="69.42578125" customWidth="1"/>
+    <col min="11" max="11" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:11" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="I1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="150" x14ac:dyDescent="0.25">
+      <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="B2" s="7" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" ht="165" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="C2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C3" t="s">
+      <c r="H3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I3" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" s="1" t="s">
+      <c r="J3" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H3" t="s">
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="B4" s="7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+      <c r="C4" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="D4" s="5"/>
+      <c r="E4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C4" t="s">
+      <c r="H4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J4" s="5"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="1" t="s">
+      <c r="B5" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="G4" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+      <c r="C5" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="D5" s="5"/>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G5" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" t="s">
+      <c r="H5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="J5" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="G5" t="s">
-        <v>14</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-      <c r="I5" s="1" t="s">
+      <c r="B6" s="7" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="F6" s="7" t="s">
         <v>33</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2" t="s">
+      <c r="G6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="H6" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="I6" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="2" t="s">
+      <c r="J6" s="7"/>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="B7" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="135" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="F7" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2" t="s">
+      <c r="G7" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="H7" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="I7" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="J7" s="7"/>
+      <c r="K7" s="6"/>
+    </row>
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
+      <c r="A8" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="150" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="F8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2" t="s">
+      <c r="H8" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="E8" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F8" s="2" t="s">
+      <c r="J8" s="7"/>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" ht="240" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H8" s="2" t="s">
+      <c r="B9" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="240" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="F9" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2" t="s">
+      <c r="G9" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="H9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I9" s="7" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="2" t="s">
+      <c r="J9" s="7"/>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H9" s="2" t="s">
+      <c r="B10" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="D10" s="7"/>
+      <c r="E10" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F10" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="2" t="s">
+      <c r="G10" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E10" s="2" t="s">
+      <c r="H10" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I10" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="J10" s="7"/>
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H10" s="2" t="s">
+      <c r="B11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="D11" s="7"/>
+      <c r="E11" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="285" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E11" s="2" t="s">
+      <c r="H11" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="I11" s="7" t="s">
         <v>61</v>
       </c>
-      <c r="G11" s="2" t="s">
+      <c r="J11" s="7"/>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="H11" s="2" t="s">
+      <c r="B12" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C12" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="D12" s="7"/>
+      <c r="E12" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F12" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C12" s="2" t="s">
+      <c r="H12" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I12" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="F12" s="2" t="s">
+      <c r="J12" s="7"/>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="H12" s="2" t="s">
+      <c r="B13" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="D13" s="7"/>
+      <c r="E13" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F13" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="B13" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C13" s="2" t="s">
+      <c r="G13" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E13" s="2" t="s">
+      <c r="H13" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I13" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="F13" s="2" t="s">
+      <c r="J13" s="7"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H13" s="2" t="s">
+      <c r="B14" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="225" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="C14" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="D14" s="7"/>
+      <c r="E14" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="F14" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="H14" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I14" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="J14" s="7" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="H14" s="2" t="s">
+      <c r="K14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A15" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I14" s="2" t="s">
+      <c r="B15" s="7" t="s">
         <v>78</v>
+      </c>
+      <c r="C15" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="K15" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+      <c r="A16" s="7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="H16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I16" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="J16" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="K16" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D17" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E17" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I17" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K17" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="H18" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I18" s="7" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A19" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C19" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D19" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I19" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="J19" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K19" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A20" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H20" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="I20" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J20" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="K20" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A21" s="7" t="s">
+        <v>103</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>104</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I21" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="K21" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A22" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C22" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="H22" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I22" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="J22" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="K22" s="6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A23" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F23" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="I23" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="K23" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>116</v>
+      </c>
+      <c r="E24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24" s="6">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>